<commit_message>
[Report 200 Pages - Group 2.docx] Update [Tasksheet.xlsx] Update
</commit_message>
<xml_diff>
--- a/Document/Report/Tasksheet.xlsx
+++ b/Document/Report/Tasksheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="149">
   <si>
     <t>No.</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Deployment at server side</t>
   </si>
   <si>
-    <t>Setting up environment at server side</t>
-  </si>
-  <si>
     <t>Setting up environment at client side</t>
   </si>
   <si>
@@ -444,13 +441,28 @@
     <t>Delete comment</t>
   </si>
   <si>
-    <t>Search comment</t>
-  </si>
-  <si>
     <t xml:space="preserve">Comment </t>
   </si>
   <si>
     <t xml:space="preserve">Rating </t>
+  </si>
+  <si>
+    <t>Forgot password</t>
+  </si>
+  <si>
+    <t>Remember me</t>
+  </si>
+  <si>
+    <t>View patient</t>
+  </si>
+  <si>
+    <t>User Role</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Server’s requirement</t>
   </si>
 </sst>
 </file>
@@ -609,7 +621,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -676,9 +688,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="6"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -692,14 +701,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -710,14 +716,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1021,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EJ206"/>
+  <dimension ref="A1:EJ210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="C123" sqref="C123"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1049,10 +1062,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>51</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>52</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>16</v>
@@ -1060,13 +1073,13 @@
       <c r="G1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="29"/>
+      <c r="I1" s="28"/>
     </row>
     <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" s="39">
+      <c r="A2" s="37">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="34" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -1078,11 +1091,11 @@
       <c r="E2" s="1"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
-      <c r="I2" s="29"/>
+      <c r="I2" s="28"/>
     </row>
     <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="2" t="s">
         <v>24</v>
       </c>
@@ -1092,13 +1105,13 @@
       <c r="E3" s="1"/>
       <c r="F3" s="10"/>
       <c r="G3" s="12"/>
-      <c r="I3" s="29"/>
+      <c r="I3" s="28"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A4" s="41">
+      <c r="A4" s="34">
         <v>2</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="35" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1110,11 +1123,11 @@
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="12"/>
-      <c r="I4" s="29"/>
+      <c r="I4" s="28"/>
     </row>
     <row r="5" spans="1:9" ht="15.75">
-      <c r="A5" s="41"/>
-      <c r="B5" s="38"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="2" t="s">
         <v>27</v>
       </c>
@@ -1124,11 +1137,11 @@
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="12"/>
-      <c r="I5" s="29"/>
+      <c r="I5" s="28"/>
     </row>
     <row r="6" spans="1:9" ht="15.75">
-      <c r="A6" s="41"/>
-      <c r="B6" s="38"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="2" t="s">
         <v>28</v>
       </c>
@@ -1138,11 +1151,11 @@
       <c r="E6" s="1"/>
       <c r="F6" s="10"/>
       <c r="G6" s="12"/>
-      <c r="I6" s="29"/>
+      <c r="I6" s="28"/>
     </row>
     <row r="7" spans="1:9" ht="15.75">
-      <c r="A7" s="41"/>
-      <c r="B7" s="39"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1152,13 +1165,13 @@
       <c r="E7" s="1"/>
       <c r="F7" s="10"/>
       <c r="G7" s="12"/>
-      <c r="I7" s="29"/>
+      <c r="I7" s="28"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A8" s="41">
+      <c r="A8" s="34">
         <v>3</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="34" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1168,11 +1181,11 @@
       <c r="E8" s="1"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-      <c r="I8" s="29"/>
+      <c r="I8" s="28"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A9" s="41"/>
-      <c r="B9" s="41"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="26" t="s">
         <v>30</v>
       </c>
@@ -1180,11 +1193,11 @@
       <c r="E9" s="1"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="I9" s="29"/>
+      <c r="I9" s="28"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A10" s="41"/>
-      <c r="B10" s="41"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="25" t="s">
         <v>41</v>
       </c>
@@ -1194,11 +1207,11 @@
       <c r="E10" s="1"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
-      <c r="I10" s="29"/>
+      <c r="I10" s="28"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
       <c r="C11" s="25" t="s">
         <v>42</v>
       </c>
@@ -1208,39 +1221,39 @@
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
-      <c r="I11" s="29"/>
+      <c r="I11" s="28"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
-      <c r="I12" s="29"/>
+      <c r="I12" s="28"/>
     </row>
     <row r="13" spans="1:9" ht="15.75">
-      <c r="A13" s="41"/>
-      <c r="B13" s="41"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
-      <c r="I13" s="29"/>
+      <c r="I13" s="28"/>
     </row>
     <row r="14" spans="1:9" ht="15.75">
-      <c r="A14" s="41"/>
-      <c r="B14" s="41"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
       <c r="C14" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
@@ -1248,13 +1261,13 @@
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
-      <c r="I14" s="29"/>
+      <c r="I14" s="28"/>
     </row>
     <row r="15" spans="1:9" ht="15.75">
-      <c r="A15" s="41"/>
-      <c r="B15" s="41"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
       <c r="C15" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
@@ -1262,13 +1275,13 @@
       <c r="E15" s="1"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
-      <c r="I15" s="29"/>
+      <c r="I15" s="28"/>
     </row>
     <row r="16" spans="1:9" ht="15.75">
-      <c r="A16" s="41"/>
-      <c r="B16" s="41"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
@@ -1276,13 +1289,13 @@
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="I16" s="29"/>
+      <c r="I16" s="28"/>
     </row>
     <row r="17" spans="1:9" ht="15.75">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>6</v>
@@ -1290,13 +1303,13 @@
       <c r="E17" s="1"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="I17" s="29"/>
+      <c r="I17" s="28"/>
     </row>
     <row r="18" spans="1:9" ht="15.75">
-      <c r="A18" s="41"/>
-      <c r="B18" s="41"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
       <c r="C18" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
@@ -1304,13 +1317,13 @@
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="I18" s="29"/>
+      <c r="I18" s="28"/>
     </row>
     <row r="19" spans="1:9" ht="15.75">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>6</v>
@@ -1318,65 +1331,67 @@
       <c r="E19" s="1"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
-      <c r="I19" s="29"/>
+      <c r="I19" s="28"/>
     </row>
     <row r="20" spans="1:9" ht="15.75">
-      <c r="A20" s="41"/>
-      <c r="B20" s="41"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="1"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
-      <c r="I20" s="29"/>
+      <c r="I20" s="28"/>
     </row>
     <row r="21" spans="1:9" ht="15.75">
-      <c r="A21" s="41"/>
-      <c r="B21" s="41"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="34"/>
       <c r="C21" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="E21" s="1"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
-      <c r="I21" s="29"/>
+      <c r="I21" s="28"/>
     </row>
     <row r="22" spans="1:9" ht="15.75">
-      <c r="A22" s="41"/>
-      <c r="B22" s="41"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
       <c r="C22" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
-      <c r="I22" s="29"/>
+      <c r="I22" s="28"/>
     </row>
     <row r="23" spans="1:9" ht="15.75">
-      <c r="A23" s="41"/>
-      <c r="B23" s="41"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
       <c r="C23" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
-      <c r="I23" s="29"/>
+      <c r="I23" s="28"/>
     </row>
     <row r="24" spans="1:9" ht="15.75">
-      <c r="A24" s="41"/>
-      <c r="B24" s="41"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
       <c r="C24" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
@@ -1384,13 +1399,13 @@
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
-      <c r="I24" s="29"/>
+      <c r="I24" s="28"/>
     </row>
     <row r="25" spans="1:9" ht="15.75">
-      <c r="A25" s="41"/>
-      <c r="B25" s="41"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
       <c r="C25" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>6</v>
@@ -1398,13 +1413,13 @@
       <c r="E25" s="1"/>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
-      <c r="I25" s="29"/>
+      <c r="I25" s="28"/>
     </row>
     <row r="26" spans="1:9" ht="15.75">
-      <c r="A26" s="41"/>
-      <c r="B26" s="41"/>
+      <c r="A26" s="34"/>
+      <c r="B26" s="34"/>
       <c r="C26" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
@@ -1412,13 +1427,13 @@
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
-      <c r="I26" s="29"/>
+      <c r="I26" s="28"/>
     </row>
     <row r="27" spans="1:9" ht="15.75">
-      <c r="A27" s="41"/>
-      <c r="B27" s="41"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="34"/>
       <c r="C27" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>6</v>
@@ -1426,13 +1441,13 @@
       <c r="E27" s="1"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
-      <c r="I27" s="29"/>
+      <c r="I27" s="28"/>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A28" s="41"/>
-      <c r="B28" s="41"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="34"/>
       <c r="C28" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
@@ -1440,27 +1455,27 @@
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
-      <c r="I28" s="29"/>
+      <c r="I28" s="28"/>
     </row>
     <row r="29" spans="1:9" ht="15.75">
-      <c r="A29" s="41"/>
-      <c r="B29" s="41"/>
+      <c r="A29" s="34"/>
+      <c r="B29" s="34"/>
       <c r="C29" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
-      <c r="I29" s="29"/>
+      <c r="I29" s="28"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A30" s="41"/>
-      <c r="B30" s="41"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="34"/>
       <c r="C30" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
@@ -1468,13 +1483,13 @@
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
-      <c r="I30" s="31"/>
+      <c r="I30" s="30"/>
     </row>
     <row r="31" spans="1:9" ht="15.75">
-      <c r="A31" s="41"/>
-      <c r="B31" s="41"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
       <c r="C31" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>6</v>
@@ -1482,27 +1497,27 @@
       <c r="E31" s="1"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
-      <c r="I31" s="29"/>
+      <c r="I31" s="28"/>
     </row>
     <row r="32" spans="1:9" ht="15.75">
-      <c r="A32" s="41"/>
-      <c r="B32" s="41"/>
+      <c r="A32" s="34"/>
+      <c r="B32" s="34"/>
       <c r="C32" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="1"/>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
-      <c r="I32" s="29"/>
+      <c r="I32" s="28"/>
     </row>
     <row r="33" spans="1:9" ht="15.75">
-      <c r="A33" s="41"/>
-      <c r="B33" s="41"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
       <c r="C33" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>6</v>
@@ -1510,11 +1525,11 @@
       <c r="E33" s="1"/>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
-      <c r="I33" s="29"/>
+      <c r="I33" s="28"/>
     </row>
     <row r="34" spans="1:9" ht="15.75">
-      <c r="A34" s="41"/>
-      <c r="B34" s="41"/>
+      <c r="A34" s="34"/>
+      <c r="B34" s="34"/>
       <c r="C34" s="26" t="s">
         <v>31</v>
       </c>
@@ -1522,13 +1537,13 @@
       <c r="E34" s="1"/>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
-      <c r="I34" s="29"/>
+      <c r="I34" s="28"/>
     </row>
     <row r="35" spans="1:9" ht="15.75">
-      <c r="A35" s="41"/>
-      <c r="B35" s="41"/>
+      <c r="A35" s="34"/>
+      <c r="B35" s="34"/>
       <c r="C35" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
@@ -1536,13 +1551,13 @@
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
-      <c r="I35" s="32"/>
+      <c r="I35" s="31"/>
     </row>
     <row r="36" spans="1:9" ht="15.75">
-      <c r="A36" s="41"/>
-      <c r="B36" s="41"/>
+      <c r="A36" s="34"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>6</v>
@@ -1550,27 +1565,27 @@
       <c r="E36" s="1"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
-      <c r="I36" s="32"/>
+      <c r="I36" s="31"/>
     </row>
     <row r="37" spans="1:9" ht="15.75">
-      <c r="A37" s="41"/>
-      <c r="B37" s="41"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
       <c r="C37" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="1"/>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
-      <c r="I37" s="32"/>
+      <c r="I37" s="31"/>
     </row>
     <row r="38" spans="1:9" ht="15.75">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
+      <c r="A38" s="34"/>
+      <c r="B38" s="34"/>
       <c r="C38" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>6</v>
@@ -1578,27 +1593,27 @@
       <c r="E38" s="1"/>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
-      <c r="I38" s="32"/>
+      <c r="I38" s="31"/>
     </row>
     <row r="39" spans="1:9" ht="15.75">
-      <c r="A39" s="41"/>
-      <c r="B39" s="41"/>
+      <c r="A39" s="34"/>
+      <c r="B39" s="34"/>
       <c r="C39" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="1"/>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
-      <c r="I39" s="32"/>
+      <c r="I39" s="31"/>
     </row>
     <row r="40" spans="1:9" ht="15.75">
-      <c r="A40" s="41"/>
-      <c r="B40" s="41"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="34"/>
       <c r="C40" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>6</v>
@@ -1606,13 +1621,13 @@
       <c r="E40" s="1"/>
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
-      <c r="I40" s="32"/>
+      <c r="I40" s="31"/>
     </row>
     <row r="41" spans="1:9" ht="15.75">
-      <c r="A41" s="41"/>
-      <c r="B41" s="41"/>
+      <c r="A41" s="34"/>
+      <c r="B41" s="34"/>
       <c r="C41" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1" t="s">
@@ -1620,27 +1635,27 @@
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
-      <c r="I41" s="32"/>
+      <c r="I41" s="31"/>
     </row>
     <row r="42" spans="1:9" ht="15.75">
-      <c r="A42" s="41"/>
-      <c r="B42" s="41"/>
+      <c r="A42" s="34"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E42" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
-      <c r="I42" s="32"/>
+      <c r="I42" s="31"/>
     </row>
     <row r="43" spans="1:9" ht="15.75">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
@@ -1648,27 +1663,27 @@
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
-      <c r="I43" s="32"/>
+      <c r="I43" s="31"/>
     </row>
     <row r="44" spans="1:9" ht="15.75">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
-      <c r="I44" s="32"/>
+      <c r="I44" s="31"/>
     </row>
     <row r="45" spans="1:9" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1" t="s">
@@ -1676,13 +1691,13 @@
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
-      <c r="I45" s="32"/>
+      <c r="I45" s="31"/>
     </row>
     <row r="46" spans="1:9" ht="15.75">
-      <c r="A46" s="41"/>
-      <c r="B46" s="41"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="34"/>
       <c r="C46" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>6</v>
@@ -1690,13 +1705,13 @@
       <c r="E46" s="1"/>
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
-      <c r="I46" s="32"/>
+      <c r="I46" s="31"/>
     </row>
     <row r="47" spans="1:9" ht="15.75">
-      <c r="A47" s="41"/>
-      <c r="B47" s="41"/>
+      <c r="A47" s="34"/>
+      <c r="B47" s="34"/>
       <c r="C47" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
@@ -1704,13 +1719,13 @@
       </c>
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
-      <c r="I47" s="29"/>
+      <c r="I47" s="28"/>
     </row>
     <row r="48" spans="1:9" ht="15.75">
-      <c r="A48" s="41"/>
-      <c r="B48" s="41"/>
+      <c r="A48" s="34"/>
+      <c r="B48" s="34"/>
       <c r="C48" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>6</v>
@@ -1718,13 +1733,13 @@
       <c r="E48" s="1"/>
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
-      <c r="I48" s="29"/>
+      <c r="I48" s="28"/>
     </row>
     <row r="49" spans="1:9" ht="15.75">
-      <c r="A49" s="41"/>
-      <c r="B49" s="41"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="34"/>
       <c r="C49" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1" t="s">
@@ -1732,13 +1747,13 @@
       </c>
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
-      <c r="I49" s="29"/>
+      <c r="I49" s="28"/>
     </row>
     <row r="50" spans="1:9" ht="15.75">
-      <c r="A50" s="41"/>
-      <c r="B50" s="41"/>
+      <c r="A50" s="34"/>
+      <c r="B50" s="34"/>
       <c r="C50" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>6</v>
@@ -1746,11 +1761,11 @@
       <c r="E50" s="1"/>
       <c r="F50" s="10"/>
       <c r="G50" s="10"/>
-      <c r="I50" s="29"/>
+      <c r="I50" s="28"/>
     </row>
     <row r="51" spans="1:9" ht="15.75">
-      <c r="A51" s="41"/>
-      <c r="B51" s="41"/>
+      <c r="A51" s="34"/>
+      <c r="B51" s="34"/>
       <c r="C51" s="4" t="s">
         <v>32</v>
       </c>
@@ -1760,13 +1775,13 @@
       <c r="E51" s="1"/>
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
-      <c r="I51" s="29"/>
+      <c r="I51" s="28"/>
     </row>
     <row r="52" spans="1:9" ht="15.75">
-      <c r="A52" s="34">
+      <c r="A52" s="38">
         <v>4</v>
       </c>
-      <c r="B52" s="37" t="s">
+      <c r="B52" s="35" t="s">
         <v>4</v>
       </c>
       <c r="C52" s="5" t="s">
@@ -1778,13 +1793,13 @@
       <c r="E52" s="1"/>
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
-      <c r="I52" s="29"/>
+      <c r="I52" s="28"/>
     </row>
     <row r="53" spans="1:9" ht="15.75">
-      <c r="A53" s="35"/>
-      <c r="B53" s="38"/>
+      <c r="A53" s="39"/>
+      <c r="B53" s="36"/>
       <c r="C53" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>6</v>
@@ -1792,13 +1807,13 @@
       <c r="E53" s="1"/>
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
-      <c r="I53" s="29"/>
+      <c r="I53" s="28"/>
     </row>
     <row r="54" spans="1:9" ht="15.75">
-      <c r="A54" s="35"/>
-      <c r="B54" s="38"/>
+      <c r="A54" s="39"/>
+      <c r="B54" s="36"/>
       <c r="C54" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>6</v>
@@ -1806,11 +1821,11 @@
       <c r="E54" s="1"/>
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
-      <c r="I54" s="29"/>
+      <c r="I54" s="28"/>
     </row>
     <row r="55" spans="1:9" ht="15.75">
-      <c r="A55" s="35"/>
-      <c r="B55" s="38"/>
+      <c r="A55" s="39"/>
+      <c r="B55" s="36"/>
       <c r="C55" s="7" t="s">
         <v>9</v>
       </c>
@@ -1820,11 +1835,11 @@
       <c r="E55" s="1"/>
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>
-      <c r="I55" s="31"/>
+      <c r="I55" s="30"/>
     </row>
     <row r="56" spans="1:9" ht="15.75">
-      <c r="A56" s="35"/>
-      <c r="B56" s="38"/>
+      <c r="A56" s="39"/>
+      <c r="B56" s="36"/>
       <c r="C56" s="5" t="s">
         <v>10</v>
       </c>
@@ -1832,11 +1847,11 @@
       <c r="E56" s="1"/>
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
-      <c r="I56" s="31"/>
+      <c r="I56" s="30"/>
     </row>
     <row r="57" spans="1:9" ht="15.75">
-      <c r="A57" s="35"/>
-      <c r="B57" s="38"/>
+      <c r="A57" s="39"/>
+      <c r="B57" s="36"/>
       <c r="C57" s="6" t="s">
         <v>34</v>
       </c>
@@ -1846,11 +1861,11 @@
       </c>
       <c r="F57" s="10"/>
       <c r="G57" s="10"/>
-      <c r="I57" s="31"/>
+      <c r="I57" s="30"/>
     </row>
     <row r="58" spans="1:9" ht="15.75">
-      <c r="A58" s="35"/>
-      <c r="B58" s="38"/>
+      <c r="A58" s="39"/>
+      <c r="B58" s="36"/>
       <c r="C58" s="22" t="s">
         <v>35</v>
       </c>
@@ -1858,27 +1873,27 @@
       <c r="E58" s="1"/>
       <c r="F58" s="10"/>
       <c r="G58" s="10"/>
-      <c r="I58" s="31"/>
+      <c r="I58" s="30"/>
     </row>
     <row r="59" spans="1:9" ht="15.75">
-      <c r="A59" s="35"/>
-      <c r="B59" s="38"/>
+      <c r="A59" s="39"/>
+      <c r="B59" s="36"/>
       <c r="C59" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F59" s="10"/>
       <c r="G59" s="10"/>
-      <c r="I59" s="31"/>
+      <c r="I59" s="30"/>
     </row>
     <row r="60" spans="1:9" ht="15.75">
-      <c r="A60" s="35"/>
-      <c r="B60" s="38"/>
+      <c r="A60" s="39"/>
+      <c r="B60" s="36"/>
       <c r="C60" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1" t="s">
@@ -1886,27 +1901,27 @@
       </c>
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
-      <c r="I60" s="31"/>
+      <c r="I60" s="30"/>
     </row>
     <row r="61" spans="1:9" ht="15.75">
-      <c r="A61" s="35"/>
-      <c r="B61" s="38"/>
+      <c r="A61" s="39"/>
+      <c r="B61" s="36"/>
       <c r="C61" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E61" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F61" s="10"/>
       <c r="G61" s="10"/>
-      <c r="I61" s="31"/>
+      <c r="I61" s="30"/>
     </row>
     <row r="62" spans="1:9" ht="15.75">
-      <c r="A62" s="35"/>
-      <c r="B62" s="38"/>
+      <c r="A62" s="39"/>
+      <c r="B62" s="36"/>
       <c r="C62" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1" t="s">
@@ -1914,27 +1929,27 @@
       </c>
       <c r="F62" s="10"/>
       <c r="G62" s="10"/>
-      <c r="I62" s="31"/>
+      <c r="I62" s="30"/>
     </row>
     <row r="63" spans="1:9" ht="15.75">
-      <c r="A63" s="35"/>
-      <c r="B63" s="38"/>
+      <c r="A63" s="39"/>
+      <c r="B63" s="36"/>
       <c r="C63" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E63" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F63" s="10"/>
       <c r="G63" s="10"/>
-      <c r="I63" s="31"/>
+      <c r="I63" s="30"/>
     </row>
     <row r="64" spans="1:9" ht="15.75">
-      <c r="A64" s="35"/>
-      <c r="B64" s="38"/>
+      <c r="A64" s="39"/>
+      <c r="B64" s="36"/>
       <c r="C64" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1" t="s">
@@ -1942,27 +1957,27 @@
       </c>
       <c r="F64" s="10"/>
       <c r="G64" s="10"/>
-      <c r="I64" s="31"/>
+      <c r="I64" s="30"/>
     </row>
     <row r="65" spans="1:9" ht="15.75">
-      <c r="A65" s="35"/>
-      <c r="B65" s="38"/>
+      <c r="A65" s="39"/>
+      <c r="B65" s="36"/>
       <c r="C65" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E65" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F65" s="10"/>
       <c r="G65" s="10"/>
-      <c r="I65" s="31"/>
+      <c r="I65" s="30"/>
     </row>
     <row r="66" spans="1:9" ht="15.75">
-      <c r="A66" s="35"/>
-      <c r="B66" s="38"/>
+      <c r="A66" s="39"/>
+      <c r="B66" s="36"/>
       <c r="C66" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1" t="s">
@@ -1970,27 +1985,27 @@
       </c>
       <c r="F66" s="10"/>
       <c r="G66" s="10"/>
-      <c r="I66" s="31"/>
+      <c r="I66" s="30"/>
     </row>
     <row r="67" spans="1:9" ht="15.75">
-      <c r="A67" s="35"/>
-      <c r="B67" s="38"/>
+      <c r="A67" s="39"/>
+      <c r="B67" s="36"/>
       <c r="C67" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E67" s="1"/>
+        <v>84</v>
+      </c>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F67" s="10"/>
       <c r="G67" s="10"/>
-      <c r="I67" s="31"/>
+      <c r="I67" s="30"/>
     </row>
     <row r="68" spans="1:9" ht="15.75">
-      <c r="A68" s="35"/>
-      <c r="B68" s="38"/>
+      <c r="A68" s="39"/>
+      <c r="B68" s="36"/>
       <c r="C68" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1" t="s">
@@ -1998,41 +2013,41 @@
       </c>
       <c r="F68" s="10"/>
       <c r="G68" s="10"/>
-      <c r="I68" s="31"/>
+      <c r="I68" s="30"/>
     </row>
     <row r="69" spans="1:9" ht="15.75">
-      <c r="A69" s="35"/>
-      <c r="B69" s="38"/>
+      <c r="A69" s="39"/>
+      <c r="B69" s="36"/>
       <c r="C69" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E69" s="1"/>
+        <v>86</v>
+      </c>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F69" s="10"/>
       <c r="G69" s="10"/>
-      <c r="I69" s="31"/>
+      <c r="I69" s="30"/>
     </row>
     <row r="70" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A70" s="35"/>
-      <c r="B70" s="38"/>
+      <c r="A70" s="39"/>
+      <c r="B70" s="36"/>
       <c r="C70" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70" s="1"/>
       <c r="F70" s="10"/>
       <c r="G70" s="10"/>
-      <c r="I70" s="31"/>
+      <c r="I70" s="30"/>
     </row>
     <row r="71" spans="1:9" ht="15.75">
-      <c r="A71" s="35"/>
-      <c r="B71" s="38"/>
+      <c r="A71" s="39"/>
+      <c r="B71" s="36"/>
       <c r="C71" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>6</v>
@@ -2040,27 +2055,27 @@
       <c r="E71" s="1"/>
       <c r="F71" s="10"/>
       <c r="G71" s="10"/>
-      <c r="I71" s="31"/>
+      <c r="I71" s="30"/>
     </row>
     <row r="72" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A72" s="35"/>
-      <c r="B72" s="38"/>
+      <c r="A72" s="39"/>
+      <c r="B72" s="36"/>
       <c r="C72" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72" s="1"/>
       <c r="F72" s="10"/>
       <c r="G72" s="10"/>
-      <c r="I72" s="31"/>
+      <c r="I72" s="30"/>
     </row>
     <row r="73" spans="1:9" ht="15.75">
-      <c r="A73" s="35"/>
-      <c r="B73" s="38"/>
+      <c r="A73" s="39"/>
+      <c r="B73" s="36"/>
       <c r="C73" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>6</v>
@@ -2068,27 +2083,27 @@
       <c r="E73" s="1"/>
       <c r="F73" s="10"/>
       <c r="G73" s="10"/>
-      <c r="I73" s="31"/>
+      <c r="I73" s="30"/>
     </row>
     <row r="74" spans="1:9" ht="15.75">
-      <c r="A74" s="35"/>
-      <c r="B74" s="38"/>
+      <c r="A74" s="39"/>
+      <c r="B74" s="36"/>
       <c r="C74" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" s="1"/>
       <c r="F74" s="10"/>
       <c r="G74" s="10"/>
-      <c r="I74" s="31"/>
+      <c r="I74" s="30"/>
     </row>
     <row r="75" spans="1:9" ht="15.75">
-      <c r="A75" s="35"/>
-      <c r="B75" s="38"/>
+      <c r="A75" s="39"/>
+      <c r="B75" s="36"/>
       <c r="C75" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>6</v>
@@ -2096,27 +2111,27 @@
       <c r="E75" s="1"/>
       <c r="F75" s="10"/>
       <c r="G75" s="10"/>
-      <c r="I75" s="31"/>
+      <c r="I75" s="30"/>
     </row>
     <row r="76" spans="1:9" ht="15.75">
-      <c r="A76" s="35"/>
-      <c r="B76" s="38"/>
+      <c r="A76" s="39"/>
+      <c r="B76" s="36"/>
       <c r="C76" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76" s="1"/>
       <c r="F76" s="10"/>
       <c r="G76" s="10"/>
-      <c r="I76" s="31"/>
+      <c r="I76" s="30"/>
     </row>
     <row r="77" spans="1:9" ht="15.75">
-      <c r="A77" s="35"/>
-      <c r="B77" s="38"/>
+      <c r="A77" s="39"/>
+      <c r="B77" s="36"/>
       <c r="C77" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>6</v>
@@ -2124,39 +2139,41 @@
       <c r="E77" s="1"/>
       <c r="F77" s="10"/>
       <c r="G77" s="10"/>
-      <c r="I77" s="31"/>
+      <c r="I77" s="30"/>
     </row>
     <row r="78" spans="1:9" ht="15.75">
-      <c r="A78" s="35"/>
-      <c r="B78" s="38"/>
+      <c r="A78" s="39"/>
+      <c r="B78" s="36"/>
       <c r="C78" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78" s="1"/>
       <c r="F78" s="10"/>
       <c r="G78" s="10"/>
-      <c r="I78" s="31"/>
+      <c r="I78" s="30"/>
     </row>
     <row r="79" spans="1:9" ht="15.75">
-      <c r="A79" s="35"/>
-      <c r="B79" s="38"/>
-      <c r="C79" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D79" s="1"/>
+      <c r="A79" s="39"/>
+      <c r="B79" s="36"/>
+      <c r="C79" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="E79" s="1"/>
       <c r="F79" s="10"/>
       <c r="G79" s="10"/>
-      <c r="I79" s="31"/>
+      <c r="I79" s="30"/>
     </row>
     <row r="80" spans="1:9" ht="15.75">
-      <c r="A80" s="35"/>
-      <c r="B80" s="38"/>
+      <c r="A80" s="39"/>
+      <c r="B80" s="36"/>
       <c r="C80" s="18" t="s">
-        <v>41</v>
+        <v>147</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>6</v>
@@ -2164,27 +2181,25 @@
       <c r="E80" s="1"/>
       <c r="F80" s="10"/>
       <c r="G80" s="10"/>
-      <c r="I80" s="31"/>
+      <c r="I80" s="30"/>
     </row>
     <row r="81" spans="1:9" ht="15.75">
-      <c r="A81" s="35"/>
-      <c r="B81" s="38"/>
-      <c r="C81" s="18" t="s">
-        <v>42</v>
+      <c r="A81" s="39"/>
+      <c r="B81" s="36"/>
+      <c r="C81" s="19" t="s">
+        <v>11</v>
       </c>
       <c r="D81" s="1"/>
-      <c r="E81" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="E81" s="1"/>
       <c r="F81" s="10"/>
       <c r="G81" s="10"/>
-      <c r="I81" s="31"/>
+      <c r="I81" s="30"/>
     </row>
     <row r="82" spans="1:9" ht="15.75">
-      <c r="A82" s="35"/>
-      <c r="B82" s="38"/>
+      <c r="A82" s="39"/>
+      <c r="B82" s="36"/>
       <c r="C82" s="18" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>6</v>
@@ -2192,13 +2207,13 @@
       <c r="E82" s="1"/>
       <c r="F82" s="10"/>
       <c r="G82" s="10"/>
-      <c r="I82" s="31"/>
+      <c r="I82" s="30"/>
     </row>
     <row r="83" spans="1:9" ht="15.75">
-      <c r="A83" s="35"/>
-      <c r="B83" s="38"/>
+      <c r="A83" s="39"/>
+      <c r="B83" s="36"/>
       <c r="C83" s="18" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1" t="s">
@@ -2206,27 +2221,27 @@
       </c>
       <c r="F83" s="10"/>
       <c r="G83" s="10"/>
-      <c r="I83" s="31"/>
+      <c r="I83" s="30"/>
     </row>
     <row r="84" spans="1:9" ht="15.75">
-      <c r="A84" s="35"/>
-      <c r="B84" s="38"/>
+      <c r="A84" s="39"/>
+      <c r="B84" s="36"/>
       <c r="C84" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E84" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F84" s="10"/>
       <c r="G84" s="10"/>
-      <c r="I84" s="31"/>
+      <c r="I84" s="30"/>
     </row>
     <row r="85" spans="1:9" ht="15.75">
-      <c r="A85" s="35"/>
-      <c r="B85" s="38"/>
+      <c r="A85" s="39"/>
+      <c r="B85" s="36"/>
       <c r="C85" s="18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1" t="s">
@@ -2234,41 +2249,41 @@
       </c>
       <c r="F85" s="10"/>
       <c r="G85" s="10"/>
-      <c r="I85" s="31"/>
+      <c r="I85" s="30"/>
     </row>
     <row r="86" spans="1:9" ht="15.75">
-      <c r="A86" s="35"/>
-      <c r="B86" s="38"/>
+      <c r="A86" s="39"/>
+      <c r="B86" s="36"/>
       <c r="C86" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E86" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F86" s="10"/>
       <c r="G86" s="10"/>
-      <c r="I86" s="31"/>
+      <c r="I86" s="30"/>
     </row>
     <row r="87" spans="1:9" ht="15.75">
-      <c r="A87" s="35"/>
-      <c r="B87" s="38"/>
+      <c r="A87" s="39"/>
+      <c r="B87" s="36"/>
       <c r="C87" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E87" s="1"/>
       <c r="F87" s="10"/>
       <c r="G87" s="10"/>
-      <c r="I87" s="31"/>
+      <c r="I87" s="30"/>
     </row>
     <row r="88" spans="1:9" ht="15.75">
-      <c r="A88" s="35"/>
-      <c r="B88" s="38"/>
+      <c r="A88" s="39"/>
+      <c r="B88" s="36"/>
       <c r="C88" s="18" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>6</v>
@@ -2276,13 +2291,13 @@
       <c r="E88" s="1"/>
       <c r="F88" s="10"/>
       <c r="G88" s="10"/>
-      <c r="I88" s="31"/>
+      <c r="I88" s="30"/>
     </row>
     <row r="89" spans="1:9" ht="15.75">
-      <c r="A89" s="35"/>
-      <c r="B89" s="38"/>
+      <c r="A89" s="39"/>
+      <c r="B89" s="36"/>
       <c r="C89" s="18" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="1" t="s">
@@ -2290,13 +2305,13 @@
       </c>
       <c r="F89" s="10"/>
       <c r="G89" s="10"/>
-      <c r="I89" s="31"/>
+      <c r="I89" s="30"/>
     </row>
     <row r="90" spans="1:9" ht="15.75">
-      <c r="A90" s="35"/>
-      <c r="B90" s="38"/>
-      <c r="C90" s="28" t="s">
-        <v>65</v>
+      <c r="A90" s="39"/>
+      <c r="B90" s="36"/>
+      <c r="C90" s="18" t="s">
+        <v>76</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>6</v>
@@ -2304,27 +2319,27 @@
       <c r="E90" s="1"/>
       <c r="F90" s="10"/>
       <c r="G90" s="10"/>
-      <c r="I90" s="31"/>
+      <c r="I90" s="30"/>
     </row>
     <row r="91" spans="1:9" ht="15.75">
-      <c r="A91" s="35"/>
-      <c r="B91" s="38"/>
-      <c r="C91" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="D91" s="1"/>
-      <c r="E91" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A91" s="39"/>
+      <c r="B91" s="36"/>
+      <c r="C91" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91" s="1"/>
       <c r="F91" s="10"/>
       <c r="G91" s="10"/>
-      <c r="I91" s="31"/>
+      <c r="I91" s="30"/>
     </row>
     <row r="92" spans="1:9" ht="15.75">
-      <c r="A92" s="35"/>
-      <c r="B92" s="38"/>
-      <c r="C92" s="28" t="s">
-        <v>99</v>
+      <c r="A92" s="39"/>
+      <c r="B92" s="36"/>
+      <c r="C92" s="43" t="s">
+        <v>64</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>6</v>
@@ -2332,13 +2347,13 @@
       <c r="E92" s="1"/>
       <c r="F92" s="10"/>
       <c r="G92" s="10"/>
-      <c r="I92" s="31"/>
+      <c r="I92" s="30"/>
     </row>
     <row r="93" spans="1:9" ht="15.75">
-      <c r="A93" s="35"/>
-      <c r="B93" s="38"/>
-      <c r="C93" s="28" t="s">
-        <v>100</v>
+      <c r="A93" s="39"/>
+      <c r="B93" s="36"/>
+      <c r="C93" s="43" t="s">
+        <v>54</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93" s="1" t="s">
@@ -2346,53 +2361,53 @@
       </c>
       <c r="F93" s="10"/>
       <c r="G93" s="10"/>
-      <c r="I93" s="31"/>
+      <c r="I93" s="30"/>
     </row>
     <row r="94" spans="1:9" ht="15.75">
-      <c r="A94" s="35"/>
-      <c r="B94" s="38"/>
-      <c r="C94" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D94" s="1"/>
+      <c r="A94" s="39"/>
+      <c r="B94" s="36"/>
+      <c r="C94" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="E94" s="1"/>
       <c r="F94" s="10"/>
       <c r="G94" s="10"/>
-      <c r="I94" s="31"/>
+      <c r="I94" s="30"/>
     </row>
     <row r="95" spans="1:9" ht="15.75">
-      <c r="A95" s="35"/>
-      <c r="B95" s="38"/>
-      <c r="C95" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="D95" s="1"/>
-      <c r="E95" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A95" s="39"/>
+      <c r="B95" s="36"/>
+      <c r="C95" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E95" s="1"/>
       <c r="F95" s="10"/>
       <c r="G95" s="10"/>
-      <c r="I95" s="31"/>
+      <c r="I95" s="30"/>
     </row>
     <row r="96" spans="1:9" ht="15.75">
-      <c r="A96" s="35"/>
-      <c r="B96" s="38"/>
-      <c r="C96" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A96" s="39"/>
+      <c r="B96" s="36"/>
+      <c r="C96" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="10"/>
       <c r="G96" s="10"/>
-      <c r="I96" s="31"/>
+      <c r="I96" s="30"/>
     </row>
     <row r="97" spans="1:9" ht="15.75">
-      <c r="A97" s="35"/>
-      <c r="B97" s="38"/>
+      <c r="A97" s="39"/>
+      <c r="B97" s="36"/>
       <c r="C97" s="21" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1" t="s">
@@ -2400,13 +2415,13 @@
       </c>
       <c r="F97" s="10"/>
       <c r="G97" s="10"/>
-      <c r="I97" s="31"/>
+      <c r="I97" s="30"/>
     </row>
     <row r="98" spans="1:9" ht="15.75">
-      <c r="A98" s="35"/>
-      <c r="B98" s="38"/>
+      <c r="A98" s="39"/>
+      <c r="B98" s="36"/>
       <c r="C98" s="21" t="s">
-        <v>102</v>
+        <v>38</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>6</v>
@@ -2414,25 +2429,27 @@
       <c r="E98" s="1"/>
       <c r="F98" s="10"/>
       <c r="G98" s="10"/>
-      <c r="I98" s="31"/>
+      <c r="I98" s="30"/>
     </row>
     <row r="99" spans="1:9" ht="15.75">
-      <c r="A99" s="35"/>
-      <c r="B99" s="38"/>
-      <c r="C99" s="20" t="s">
-        <v>39</v>
+      <c r="A99" s="39"/>
+      <c r="B99" s="36"/>
+      <c r="C99" s="21" t="s">
+        <v>100</v>
       </c>
       <c r="D99" s="1"/>
-      <c r="E99" s="1"/>
+      <c r="E99" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F99" s="10"/>
       <c r="G99" s="10"/>
-      <c r="I99" s="31"/>
+      <c r="I99" s="30"/>
     </row>
     <row r="100" spans="1:9" ht="15.75">
-      <c r="A100" s="35"/>
-      <c r="B100" s="39"/>
+      <c r="A100" s="39"/>
+      <c r="B100" s="36"/>
       <c r="C100" s="21" t="s">
-        <v>40</v>
+        <v>101</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>6</v>
@@ -2440,269 +2457,263 @@
       <c r="E100" s="1"/>
       <c r="F100" s="10"/>
       <c r="G100" s="10"/>
-      <c r="I100" s="31"/>
-    </row>
-    <row r="101" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A101" s="34">
-        <v>5</v>
-      </c>
-      <c r="B101" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="C101" s="24" t="s">
-        <v>40</v>
+      <c r="I100" s="30"/>
+    </row>
+    <row r="101" spans="1:9" ht="15.75">
+      <c r="A101" s="39"/>
+      <c r="B101" s="36"/>
+      <c r="C101" s="20" t="s">
+        <v>39</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="10"/>
       <c r="G101" s="10"/>
-      <c r="I101" s="31"/>
+      <c r="I101" s="30"/>
     </row>
     <row r="102" spans="1:9" ht="15.75">
-      <c r="A102" s="35"/>
-      <c r="B102" s="38"/>
-      <c r="C102" s="6" t="s">
-        <v>41</v>
+      <c r="A102" s="39"/>
+      <c r="B102" s="37"/>
+      <c r="C102" s="21" t="s">
+        <v>40</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="10"/>
-      <c r="G102" s="10">
-        <v>1</v>
-      </c>
-      <c r="I102" s="31"/>
-    </row>
-    <row r="103" spans="1:9" ht="15.75">
-      <c r="A103" s="35"/>
-      <c r="B103" s="38"/>
-      <c r="C103" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="G102" s="10"/>
+      <c r="I102" s="30"/>
+    </row>
+    <row r="103" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A103" s="38">
+        <v>5</v>
+      </c>
+      <c r="B103" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C103" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D103" s="1"/>
       <c r="E103" s="1"/>
       <c r="F103" s="10"/>
-      <c r="G103" s="10">
-        <v>1</v>
-      </c>
-      <c r="I103" s="31"/>
+      <c r="G103" s="10"/>
+      <c r="I103" s="30"/>
     </row>
     <row r="104" spans="1:9" ht="15.75">
-      <c r="A104" s="35"/>
-      <c r="B104" s="38"/>
+      <c r="A104" s="39"/>
+      <c r="B104" s="36"/>
       <c r="C104" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E104" s="1"/>
       <c r="F104" s="10"/>
       <c r="G104" s="10">
         <v>1</v>
       </c>
-      <c r="I104" s="31"/>
+      <c r="I104" s="30"/>
     </row>
     <row r="105" spans="1:9" ht="15.75">
-      <c r="A105" s="35"/>
-      <c r="B105" s="38"/>
+      <c r="A105" s="39"/>
+      <c r="B105" s="36"/>
       <c r="C105" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D105" s="1"/>
-      <c r="E105" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E105" s="1"/>
       <c r="F105" s="10"/>
       <c r="G105" s="10">
         <v>1</v>
       </c>
-      <c r="I105" s="29"/>
-    </row>
-    <row r="106" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A106" s="35"/>
-      <c r="B106" s="38"/>
+      <c r="I105" s="30"/>
+    </row>
+    <row r="106" spans="1:9" ht="15.75">
+      <c r="A106" s="39"/>
+      <c r="B106" s="36"/>
       <c r="C106" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D106" s="1"/>
-      <c r="E106" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E106" s="1"/>
       <c r="F106" s="10"/>
       <c r="G106" s="10">
-        <v>2</v>
-      </c>
-      <c r="I106" s="29"/>
+        <v>1</v>
+      </c>
+      <c r="I106" s="30"/>
     </row>
     <row r="107" spans="1:9" ht="15.75">
-      <c r="A107" s="35"/>
-      <c r="B107" s="38"/>
+      <c r="A107" s="39"/>
+      <c r="B107" s="36"/>
       <c r="C107" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E107" s="1"/>
-      <c r="F107" s="12"/>
+        <v>143</v>
+      </c>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F107" s="10"/>
       <c r="G107" s="10">
         <v>1</v>
       </c>
-      <c r="I107" s="29"/>
+      <c r="I107" s="30"/>
     </row>
     <row r="108" spans="1:9" ht="15.75">
-      <c r="A108" s="35"/>
-      <c r="B108" s="38"/>
+      <c r="A108" s="39"/>
+      <c r="B108" s="36"/>
       <c r="C108" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E108" s="1"/>
-      <c r="F108" s="12"/>
+        <v>42</v>
+      </c>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F108" s="10"/>
       <c r="G108" s="10">
         <v>1</v>
       </c>
-      <c r="I108" s="29"/>
+      <c r="I108" s="30"/>
     </row>
     <row r="109" spans="1:9" ht="15.75">
-      <c r="A109" s="35"/>
-      <c r="B109" s="38"/>
+      <c r="A109" s="39"/>
+      <c r="B109" s="36"/>
       <c r="C109" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E109" s="1"/>
+        <v>103</v>
+      </c>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F109" s="10"/>
       <c r="G109" s="10">
         <v>1</v>
       </c>
-      <c r="I109" s="29"/>
-    </row>
-    <row r="110" spans="1:9" ht="15.75">
-      <c r="A110" s="35"/>
-      <c r="B110" s="38"/>
+      <c r="I109" s="28"/>
+    </row>
+    <row r="110" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A110" s="39"/>
+      <c r="B110" s="36"/>
       <c r="C110" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E110" s="1"/>
+        <v>104</v>
+      </c>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F110" s="10"/>
       <c r="G110" s="10">
-        <v>1</v>
-      </c>
-      <c r="I110" s="29"/>
+        <v>2</v>
+      </c>
+      <c r="I110" s="28"/>
     </row>
     <row r="111" spans="1:9" ht="15.75">
-      <c r="A111" s="35"/>
-      <c r="B111" s="38"/>
+      <c r="A111" s="39"/>
+      <c r="B111" s="36"/>
       <c r="C111" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E111" s="1"/>
-      <c r="F111" s="10"/>
+      <c r="F111" s="12"/>
       <c r="G111" s="10">
         <v>1</v>
       </c>
-      <c r="I111" s="29"/>
+      <c r="I111" s="28"/>
     </row>
     <row r="112" spans="1:9" ht="15.75">
-      <c r="A112" s="35"/>
-      <c r="B112" s="38"/>
+      <c r="A112" s="39"/>
+      <c r="B112" s="36"/>
       <c r="C112" s="6" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E112" s="1"/>
-      <c r="F112" s="10"/>
+      <c r="F112" s="12"/>
       <c r="G112" s="10">
         <v>1</v>
       </c>
-      <c r="I112" s="29"/>
+      <c r="I112" s="28"/>
     </row>
     <row r="113" spans="1:9" ht="15.75">
-      <c r="A113" s="35"/>
-      <c r="B113" s="38"/>
+      <c r="A113" s="39"/>
+      <c r="B113" s="36"/>
       <c r="C113" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D113" s="1"/>
-      <c r="E113" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E113" s="1"/>
       <c r="F113" s="10"/>
       <c r="G113" s="10">
-        <v>2</v>
-      </c>
-      <c r="I113" s="29"/>
+        <v>1</v>
+      </c>
+      <c r="I113" s="28"/>
     </row>
     <row r="114" spans="1:9" ht="15.75">
-      <c r="A114" s="35"/>
-      <c r="B114" s="38"/>
+      <c r="A114" s="39"/>
+      <c r="B114" s="36"/>
       <c r="C114" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D114" s="1"/>
-      <c r="E114" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E114" s="1"/>
       <c r="F114" s="10"/>
       <c r="G114" s="10">
         <v>1</v>
       </c>
-      <c r="I114" s="29"/>
+      <c r="I114" s="28"/>
     </row>
     <row r="115" spans="1:9" ht="15.75">
-      <c r="A115" s="35"/>
-      <c r="B115" s="38"/>
+      <c r="A115" s="39"/>
+      <c r="B115" s="36"/>
       <c r="C115" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D115" s="1"/>
-      <c r="E115" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E115" s="1"/>
       <c r="F115" s="10"/>
       <c r="G115" s="10">
-        <v>2</v>
-      </c>
-      <c r="I115" s="29"/>
+        <v>1</v>
+      </c>
+      <c r="I115" s="28"/>
     </row>
     <row r="116" spans="1:9" ht="15.75">
-      <c r="A116" s="35"/>
-      <c r="B116" s="38"/>
+      <c r="A116" s="39"/>
+      <c r="B116" s="36"/>
       <c r="C116" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D116" s="1"/>
-      <c r="E116" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E116" s="1"/>
       <c r="F116" s="10"/>
       <c r="G116" s="10">
         <v>1</v>
       </c>
-      <c r="I116" s="29"/>
+      <c r="I116" s="28"/>
     </row>
     <row r="117" spans="1:9" ht="15.75">
-      <c r="A117" s="35"/>
-      <c r="B117" s="38"/>
+      <c r="A117" s="39"/>
+      <c r="B117" s="36"/>
       <c r="C117" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D117" s="1"/>
       <c r="E117" s="1" t="s">
@@ -2710,15 +2721,15 @@
       </c>
       <c r="F117" s="10"/>
       <c r="G117" s="10">
-        <v>1</v>
-      </c>
-      <c r="I117" s="29"/>
+        <v>2</v>
+      </c>
+      <c r="I117" s="28"/>
     </row>
     <row r="118" spans="1:9" ht="15.75">
-      <c r="A118" s="35"/>
-      <c r="B118" s="38"/>
+      <c r="A118" s="39"/>
+      <c r="B118" s="36"/>
       <c r="C118" s="6" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="D118" s="1"/>
       <c r="E118" s="1" t="s">
@@ -2728,45 +2739,45 @@
       <c r="G118" s="10">
         <v>1</v>
       </c>
-      <c r="I118" s="29"/>
+      <c r="I118" s="28"/>
     </row>
     <row r="119" spans="1:9" ht="15.75">
-      <c r="A119" s="35"/>
-      <c r="B119" s="38"/>
+      <c r="A119" s="39"/>
+      <c r="B119" s="36"/>
       <c r="C119" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E119" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="D119" s="1"/>
+      <c r="E119" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F119" s="10"/>
       <c r="G119" s="10">
-        <v>3</v>
-      </c>
-      <c r="I119" s="29"/>
+        <v>2</v>
+      </c>
+      <c r="I119" s="28"/>
     </row>
     <row r="120" spans="1:9" ht="15.75">
-      <c r="A120" s="35"/>
-      <c r="B120" s="38"/>
+      <c r="A120" s="39"/>
+      <c r="B120" s="36"/>
       <c r="C120" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E120" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="D120" s="1"/>
+      <c r="E120" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F120" s="10"/>
       <c r="G120" s="10">
-        <v>3</v>
-      </c>
-      <c r="I120" s="30"/>
+        <v>1</v>
+      </c>
+      <c r="I120" s="28"/>
     </row>
     <row r="121" spans="1:9" ht="15.75">
-      <c r="A121" s="35"/>
-      <c r="B121" s="38"/>
+      <c r="A121" s="39"/>
+      <c r="B121" s="36"/>
       <c r="C121" s="6" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="1" t="s">
@@ -2774,15 +2785,15 @@
       </c>
       <c r="F121" s="10"/>
       <c r="G121" s="10">
-        <v>3</v>
-      </c>
-      <c r="I121" s="30"/>
+        <v>1</v>
+      </c>
+      <c r="I121" s="28"/>
     </row>
     <row r="122" spans="1:9" ht="15.75">
-      <c r="A122" s="35"/>
-      <c r="B122" s="38"/>
+      <c r="A122" s="39"/>
+      <c r="B122" s="36"/>
       <c r="C122" s="6" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="1" t="s">
@@ -2790,110 +2801,110 @@
       </c>
       <c r="F122" s="10"/>
       <c r="G122" s="10">
-        <v>3</v>
-      </c>
-      <c r="I122" s="30"/>
+        <v>1</v>
+      </c>
+      <c r="I122" s="28"/>
     </row>
     <row r="123" spans="1:9" ht="15.75">
-      <c r="A123" s="35"/>
-      <c r="B123" s="38"/>
+      <c r="A123" s="39"/>
+      <c r="B123" s="36"/>
       <c r="C123" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D123" s="1"/>
-      <c r="E123" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E123" s="1"/>
       <c r="F123" s="10"/>
       <c r="G123" s="10">
-        <v>3</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="I123" s="28"/>
     </row>
     <row r="124" spans="1:9" ht="15.75">
-      <c r="A124" s="35"/>
-      <c r="B124" s="38"/>
+      <c r="A124" s="39"/>
+      <c r="B124" s="36"/>
       <c r="C124" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D124" s="1"/>
-      <c r="E124" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E124" s="1"/>
       <c r="F124" s="10"/>
       <c r="G124" s="10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I124" s="29"/>
     </row>
     <row r="125" spans="1:9" ht="15.75">
-      <c r="A125" s="35"/>
-      <c r="B125" s="38"/>
+      <c r="A125" s="39"/>
+      <c r="B125" s="36"/>
       <c r="C125" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E125" s="1"/>
+        <v>125</v>
+      </c>
+      <c r="D125" s="1"/>
+      <c r="E125" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F125" s="10"/>
       <c r="G125" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I125" s="29"/>
     </row>
     <row r="126" spans="1:9" ht="15.75">
-      <c r="A126" s="35"/>
-      <c r="B126" s="38"/>
+      <c r="A126" s="39"/>
+      <c r="B126" s="36"/>
       <c r="C126" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E126" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="D126" s="1"/>
+      <c r="E126" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F126" s="10"/>
       <c r="G126" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I126" s="29"/>
     </row>
     <row r="127" spans="1:9" ht="15.75">
-      <c r="A127" s="35"/>
-      <c r="B127" s="38"/>
+      <c r="A127" s="39"/>
+      <c r="B127" s="36"/>
       <c r="C127" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E127" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="D127" s="1"/>
+      <c r="E127" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F127" s="10"/>
       <c r="G127" s="10">
-        <v>2</v>
-      </c>
-      <c r="I127" s="29"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="128" spans="1:9" ht="15.75">
-      <c r="A128" s="35"/>
-      <c r="B128" s="38"/>
+      <c r="A128" s="39"/>
+      <c r="B128" s="36"/>
       <c r="C128" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E128" s="1"/>
+        <v>116</v>
+      </c>
+      <c r="D128" s="1"/>
+      <c r="E128" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F128" s="10"/>
       <c r="G128" s="10">
         <v>1</v>
       </c>
-      <c r="I128" s="29"/>
+      <c r="I128" s="28"/>
     </row>
     <row r="129" spans="1:9" ht="15.75">
-      <c r="A129" s="35"/>
-      <c r="B129" s="38"/>
+      <c r="A129" s="39"/>
+      <c r="B129" s="36"/>
       <c r="C129" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>6</v>
@@ -2903,13 +2914,13 @@
       <c r="G129" s="10">
         <v>1</v>
       </c>
-      <c r="I129" s="29"/>
+      <c r="I129" s="28"/>
     </row>
     <row r="130" spans="1:9" ht="15.75">
-      <c r="A130" s="35"/>
-      <c r="B130" s="38"/>
+      <c r="A130" s="39"/>
+      <c r="B130" s="36"/>
       <c r="C130" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>6</v>
@@ -2919,13 +2930,13 @@
       <c r="G130" s="10">
         <v>1</v>
       </c>
-      <c r="I130" s="29"/>
+      <c r="I130" s="28"/>
     </row>
     <row r="131" spans="1:9" ht="15.75">
-      <c r="A131" s="35"/>
-      <c r="B131" s="38"/>
+      <c r="A131" s="39"/>
+      <c r="B131" s="36"/>
       <c r="C131" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>6</v>
@@ -2935,13 +2946,13 @@
       <c r="G131" s="10">
         <v>1</v>
       </c>
-      <c r="I131" s="29"/>
+      <c r="I131" s="28"/>
     </row>
     <row r="132" spans="1:9" ht="15.75">
-      <c r="A132" s="35"/>
-      <c r="B132" s="38"/>
+      <c r="A132" s="39"/>
+      <c r="B132" s="36"/>
       <c r="C132" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>6</v>
@@ -2951,77 +2962,77 @@
       <c r="G132" s="10">
         <v>1</v>
       </c>
-      <c r="I132" s="29"/>
+      <c r="I132" s="28"/>
     </row>
     <row r="133" spans="1:9" ht="15.75">
-      <c r="A133" s="35"/>
-      <c r="B133" s="38"/>
+      <c r="A133" s="39"/>
+      <c r="B133" s="36"/>
       <c r="C133" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D133" s="1"/>
-      <c r="E133" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E133" s="1"/>
       <c r="F133" s="10"/>
       <c r="G133" s="10">
         <v>1</v>
       </c>
-      <c r="I133" s="29"/>
+      <c r="I133" s="28"/>
     </row>
     <row r="134" spans="1:9" ht="15.75">
-      <c r="A134" s="35"/>
-      <c r="B134" s="38"/>
+      <c r="A134" s="39"/>
+      <c r="B134" s="36"/>
       <c r="C134" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="D134" s="1"/>
-      <c r="E134" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E134" s="1"/>
       <c r="F134" s="10"/>
       <c r="G134" s="10">
         <v>1</v>
       </c>
-      <c r="I134" s="29"/>
+      <c r="I134" s="28"/>
     </row>
     <row r="135" spans="1:9" ht="15.75">
-      <c r="A135" s="35"/>
-      <c r="B135" s="38"/>
+      <c r="A135" s="39"/>
+      <c r="B135" s="36"/>
       <c r="C135" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D135" s="1"/>
-      <c r="E135" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E135" s="1"/>
       <c r="F135" s="10"/>
       <c r="G135" s="10">
         <v>1</v>
       </c>
-      <c r="I135" s="29"/>
+      <c r="I135" s="28"/>
     </row>
     <row r="136" spans="1:9" ht="15.75">
-      <c r="A136" s="35"/>
-      <c r="B136" s="38"/>
+      <c r="A136" s="39"/>
+      <c r="B136" s="36"/>
       <c r="C136" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D136" s="1"/>
-      <c r="E136" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E136" s="1"/>
       <c r="F136" s="10"/>
       <c r="G136" s="10">
         <v>1</v>
       </c>
-      <c r="I136" s="29"/>
+      <c r="I136" s="28"/>
     </row>
     <row r="137" spans="1:9" ht="15.75">
-      <c r="A137" s="35"/>
-      <c r="B137" s="38"/>
-      <c r="C137" s="33" t="s">
-        <v>66</v>
+      <c r="A137" s="39"/>
+      <c r="B137" s="36"/>
+      <c r="C137" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="D137" s="1"/>
       <c r="E137" s="1" t="s">
@@ -3029,14 +3040,14 @@
       </c>
       <c r="F137" s="10"/>
       <c r="G137" s="10">
-        <v>2</v>
-      </c>
-      <c r="I137" s="29"/>
+        <v>1</v>
+      </c>
+      <c r="I137" s="28"/>
     </row>
     <row r="138" spans="1:9" ht="15.75">
-      <c r="A138" s="35"/>
-      <c r="B138" s="38"/>
-      <c r="C138" s="33" t="s">
+      <c r="A138" s="39"/>
+      <c r="B138" s="36"/>
+      <c r="C138" s="6" t="s">
         <v>138</v>
       </c>
       <c r="D138" s="1"/>
@@ -3047,13 +3058,13 @@
       <c r="G138" s="10">
         <v>1</v>
       </c>
-      <c r="I138" s="29"/>
+      <c r="I138" s="28"/>
     </row>
     <row r="139" spans="1:9" ht="15.75">
-      <c r="A139" s="35"/>
-      <c r="B139" s="38"/>
-      <c r="C139" s="33" t="s">
-        <v>67</v>
+      <c r="A139" s="39"/>
+      <c r="B139" s="36"/>
+      <c r="C139" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="D139" s="1"/>
       <c r="E139" s="1" t="s">
@@ -3061,15 +3072,15 @@
       </c>
       <c r="F139" s="10"/>
       <c r="G139" s="10">
-        <v>2</v>
-      </c>
-      <c r="I139" s="29"/>
+        <v>1</v>
+      </c>
+      <c r="I139" s="28"/>
     </row>
     <row r="140" spans="1:9" ht="15.75">
-      <c r="A140" s="35"/>
-      <c r="B140" s="38"/>
-      <c r="C140" s="33" t="s">
-        <v>121</v>
+      <c r="A140" s="39"/>
+      <c r="B140" s="36"/>
+      <c r="C140" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="D140" s="1"/>
       <c r="E140" s="1" t="s">
@@ -3079,61 +3090,61 @@
       <c r="G140" s="10">
         <v>1</v>
       </c>
-      <c r="I140" s="29"/>
+      <c r="I140" s="28"/>
     </row>
     <row r="141" spans="1:9" ht="15.75">
-      <c r="A141" s="35"/>
-      <c r="B141" s="38"/>
-      <c r="C141" s="33" t="s">
-        <v>140</v>
-      </c>
-      <c r="D141" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E141" s="1"/>
+      <c r="A141" s="39"/>
+      <c r="B141" s="36"/>
+      <c r="C141" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D141" s="1"/>
+      <c r="E141" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F141" s="10"/>
       <c r="G141" s="10">
-        <v>1</v>
-      </c>
-      <c r="I141" s="29"/>
+        <v>2</v>
+      </c>
+      <c r="I141" s="28"/>
     </row>
     <row r="142" spans="1:9" ht="15.75">
-      <c r="A142" s="35"/>
-      <c r="B142" s="38"/>
-      <c r="C142" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E142" s="1"/>
+      <c r="A142" s="39"/>
+      <c r="B142" s="36"/>
+      <c r="C142" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="D142" s="1"/>
+      <c r="E142" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F142" s="10"/>
       <c r="G142" s="10">
         <v>1</v>
       </c>
-      <c r="I142" s="29"/>
+      <c r="I142" s="28"/>
     </row>
     <row r="143" spans="1:9" ht="15.75">
-      <c r="A143" s="35"/>
-      <c r="B143" s="38"/>
-      <c r="C143" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E143" s="1"/>
+      <c r="A143" s="39"/>
+      <c r="B143" s="36"/>
+      <c r="C143" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="D143" s="1"/>
+      <c r="E143" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F143" s="10"/>
       <c r="G143" s="10">
         <v>1</v>
       </c>
-      <c r="I143" s="29"/>
+      <c r="I143" s="28"/>
     </row>
     <row r="144" spans="1:9" ht="15.75">
-      <c r="A144" s="35"/>
-      <c r="B144" s="38"/>
-      <c r="C144" s="33" t="s">
-        <v>143</v>
+      <c r="A144" s="39"/>
+      <c r="B144" s="36"/>
+      <c r="C144" s="32" t="s">
+        <v>66</v>
       </c>
       <c r="D144" s="1"/>
       <c r="E144" s="1" t="s">
@@ -3143,77 +3154,77 @@
       <c r="G144" s="10">
         <v>2</v>
       </c>
-      <c r="I144" s="29"/>
+      <c r="I144" s="28"/>
     </row>
     <row r="145" spans="1:9" ht="15.75">
-      <c r="A145" s="35"/>
-      <c r="B145" s="38"/>
-      <c r="C145" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E145" s="1"/>
+      <c r="A145" s="39"/>
+      <c r="B145" s="36"/>
+      <c r="C145" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D145" s="1"/>
+      <c r="E145" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F145" s="10"/>
       <c r="G145" s="10">
-        <v>2</v>
-      </c>
-      <c r="I145" s="29"/>
+        <v>1</v>
+      </c>
+      <c r="I145" s="28"/>
     </row>
     <row r="146" spans="1:9" ht="15.75">
-      <c r="A146" s="35"/>
-      <c r="B146" s="38"/>
-      <c r="C146" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="D146" s="1"/>
-      <c r="E146" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A146" s="39"/>
+      <c r="B146" s="36"/>
+      <c r="C146" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E146" s="1"/>
       <c r="F146" s="10"/>
       <c r="G146" s="10">
-        <v>3</v>
-      </c>
-      <c r="I146" s="29"/>
+        <v>1</v>
+      </c>
+      <c r="I146" s="28"/>
     </row>
     <row r="147" spans="1:9" ht="15.75">
-      <c r="A147" s="35"/>
-      <c r="B147" s="38"/>
-      <c r="C147" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="D147" s="1"/>
-      <c r="E147" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A147" s="39"/>
+      <c r="B147" s="36"/>
+      <c r="C147" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E147" s="1"/>
       <c r="F147" s="10"/>
       <c r="G147" s="10">
-        <v>2</v>
-      </c>
-      <c r="I147" s="29"/>
+        <v>1</v>
+      </c>
+      <c r="I147" s="28"/>
     </row>
     <row r="148" spans="1:9" ht="15.75">
-      <c r="A148" s="35"/>
-      <c r="B148" s="38"/>
-      <c r="C148" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="D148" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E148" s="1"/>
+      <c r="A148" s="39"/>
+      <c r="B148" s="36"/>
+      <c r="C148" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D148" s="1"/>
+      <c r="E148" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F148" s="10"/>
       <c r="G148" s="10">
-        <v>3</v>
-      </c>
-      <c r="I148" s="29"/>
+        <v>2</v>
+      </c>
+      <c r="I148" s="28"/>
     </row>
     <row r="149" spans="1:9" ht="15.75">
-      <c r="A149" s="35"/>
-      <c r="B149" s="38"/>
-      <c r="C149" s="33" t="s">
-        <v>57</v>
+      <c r="A149" s="39"/>
+      <c r="B149" s="36"/>
+      <c r="C149" s="32" t="s">
+        <v>142</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>6</v>
@@ -3221,31 +3232,31 @@
       <c r="E149" s="1"/>
       <c r="F149" s="10"/>
       <c r="G149" s="10">
-        <v>3</v>
-      </c>
-      <c r="I149" s="29"/>
+        <v>2</v>
+      </c>
+      <c r="I149" s="28"/>
     </row>
     <row r="150" spans="1:9" ht="15.75">
-      <c r="A150" s="35"/>
-      <c r="B150" s="38"/>
-      <c r="C150" s="33" t="s">
-        <v>123</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E150" s="1"/>
+      <c r="A150" s="39"/>
+      <c r="B150" s="36"/>
+      <c r="C150" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D150" s="1"/>
+      <c r="E150" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F150" s="10"/>
       <c r="G150" s="10">
-        <v>2</v>
-      </c>
-      <c r="I150" s="29"/>
+        <v>3</v>
+      </c>
+      <c r="I150" s="28"/>
     </row>
     <row r="151" spans="1:9" ht="15.75">
-      <c r="A151" s="35"/>
-      <c r="B151" s="38"/>
-      <c r="C151" s="33" t="s">
-        <v>59</v>
+      <c r="A151" s="39"/>
+      <c r="B151" s="36"/>
+      <c r="C151" s="32" t="s">
+        <v>57</v>
       </c>
       <c r="D151" s="1"/>
       <c r="E151" s="1" t="s">
@@ -3253,294 +3264,330 @@
       </c>
       <c r="F151" s="10"/>
       <c r="G151" s="10">
-        <v>2</v>
-      </c>
-      <c r="I151" s="29"/>
+        <v>1</v>
+      </c>
+      <c r="I151" s="28"/>
     </row>
     <row r="152" spans="1:9" ht="15.75">
-      <c r="A152" s="35"/>
-      <c r="B152" s="38"/>
-      <c r="C152" s="33" t="s">
-        <v>124</v>
-      </c>
-      <c r="D152" s="1"/>
-      <c r="E152" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A152" s="39"/>
+      <c r="B152" s="36"/>
+      <c r="C152" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E152" s="1"/>
       <c r="F152" s="10"/>
       <c r="G152" s="10">
-        <v>1</v>
-      </c>
-      <c r="I152" s="29"/>
+        <v>3</v>
+      </c>
+      <c r="I152" s="28"/>
     </row>
     <row r="153" spans="1:9" ht="15.75">
-      <c r="A153" s="35"/>
-      <c r="B153" s="38"/>
-      <c r="C153" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="D153" s="1"/>
-      <c r="E153" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A153" s="39"/>
+      <c r="B153" s="36"/>
+      <c r="C153" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E153" s="1"/>
       <c r="F153" s="10"/>
       <c r="G153" s="10">
-        <v>1</v>
-      </c>
-      <c r="I153" s="29"/>
+        <v>3</v>
+      </c>
+      <c r="I153" s="28"/>
     </row>
     <row r="154" spans="1:9" ht="15.75">
-      <c r="A154" s="35"/>
-      <c r="B154" s="38"/>
-      <c r="C154" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E154" s="1"/>
+      <c r="A154" s="39"/>
+      <c r="B154" s="36"/>
+      <c r="C154" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="D154" s="1"/>
+      <c r="E154" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F154" s="10"/>
-      <c r="G154" s="10"/>
-      <c r="I154" s="29"/>
+      <c r="G154" s="10">
+        <v>2</v>
+      </c>
+      <c r="I154" s="28"/>
     </row>
     <row r="155" spans="1:9" ht="15.75">
-      <c r="A155" s="35"/>
-      <c r="B155" s="38"/>
-      <c r="C155" s="24" t="s">
-        <v>44</v>
+      <c r="A155" s="39"/>
+      <c r="B155" s="36"/>
+      <c r="C155" s="32" t="s">
+        <v>58</v>
       </c>
       <c r="D155" s="1"/>
-      <c r="E155" s="1"/>
+      <c r="E155" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F155" s="10"/>
-      <c r="G155" s="10"/>
-      <c r="I155" s="29"/>
+      <c r="G155" s="10">
+        <v>2</v>
+      </c>
+      <c r="I155" s="28"/>
     </row>
     <row r="156" spans="1:9" ht="15.75">
-      <c r="A156" s="35"/>
-      <c r="B156" s="38"/>
-      <c r="C156" s="6" t="s">
-        <v>45</v>
+      <c r="A156" s="39"/>
+      <c r="B156" s="36"/>
+      <c r="C156" s="32" t="s">
+        <v>123</v>
       </c>
       <c r="D156" s="1"/>
       <c r="E156" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F156" s="10"/>
-      <c r="G156" s="10"/>
-      <c r="I156" s="29"/>
+      <c r="G156" s="10">
+        <v>1</v>
+      </c>
+      <c r="I156" s="28"/>
     </row>
     <row r="157" spans="1:9" ht="15.75">
-      <c r="A157" s="35"/>
-      <c r="B157" s="38"/>
-      <c r="C157" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E157" s="1"/>
+      <c r="A157" s="39"/>
+      <c r="B157" s="36"/>
+      <c r="C157" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="D157" s="1"/>
+      <c r="E157" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F157" s="10"/>
-      <c r="G157" s="10"/>
-      <c r="I157" s="29"/>
+      <c r="G157" s="10">
+        <v>1</v>
+      </c>
+      <c r="I157" s="28"/>
     </row>
     <row r="158" spans="1:9" ht="15.75">
-      <c r="A158" s="35"/>
-      <c r="B158" s="38"/>
-      <c r="C158" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="D158" s="1"/>
-      <c r="E158" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A158" s="39"/>
+      <c r="B158" s="36"/>
+      <c r="C158" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E158" s="1"/>
       <c r="F158" s="10"/>
       <c r="G158" s="10"/>
-      <c r="I158" s="29"/>
+      <c r="I158" s="28"/>
     </row>
     <row r="159" spans="1:9" ht="15.75">
-      <c r="A159" s="40"/>
-      <c r="B159" s="39"/>
-      <c r="C159" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A159" s="39"/>
+      <c r="B159" s="36"/>
+      <c r="C159" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D159" s="1"/>
       <c r="E159" s="1"/>
       <c r="F159" s="10"/>
       <c r="G159" s="10"/>
-      <c r="I159" s="29"/>
+      <c r="I159" s="28"/>
     </row>
     <row r="160" spans="1:9" ht="15.75">
-      <c r="A160" s="36">
-        <v>6</v>
-      </c>
-      <c r="B160" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="C160" s="24" t="s">
-        <v>12</v>
+      <c r="A160" s="39"/>
+      <c r="B160" s="36"/>
+      <c r="C160" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="D160" s="1"/>
-      <c r="E160" s="1"/>
+      <c r="E160" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F160" s="10"/>
       <c r="G160" s="10"/>
-      <c r="I160" s="29"/>
-    </row>
-    <row r="161" spans="1:140" ht="15.75">
-      <c r="A161" s="36"/>
+      <c r="I160" s="28"/>
+    </row>
+    <row r="161" spans="1:10" ht="15.75">
+      <c r="A161" s="39"/>
       <c r="B161" s="36"/>
       <c r="C161" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D161" s="1"/>
-      <c r="E161" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E161" s="1"/>
       <c r="F161" s="10"/>
       <c r="G161" s="10"/>
-      <c r="I161" s="29"/>
-    </row>
-    <row r="162" spans="1:140" ht="15.75">
-      <c r="A162" s="36"/>
+      <c r="I161" s="28"/>
+    </row>
+    <row r="162" spans="1:10" ht="15.75">
+      <c r="A162" s="39"/>
       <c r="B162" s="36"/>
       <c r="C162" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D162" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E162" s="1"/>
+        <v>131</v>
+      </c>
+      <c r="D162" s="1"/>
+      <c r="E162" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F162" s="10"/>
       <c r="G162" s="10"/>
-      <c r="I162" s="29"/>
-    </row>
-    <row r="163" spans="1:140" ht="15.75">
-      <c r="A163" s="36"/>
-      <c r="B163" s="36"/>
-      <c r="C163" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D163" s="1"/>
+      <c r="I162" s="28"/>
+    </row>
+    <row r="163" spans="1:10" ht="15.75">
+      <c r="A163" s="41"/>
+      <c r="B163" s="37"/>
+      <c r="C163" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="E163" s="1"/>
       <c r="F163" s="10"/>
       <c r="G163" s="10"/>
-      <c r="I163" s="29"/>
-    </row>
-    <row r="164" spans="1:140" ht="15.75">
-      <c r="A164" s="36"/>
-      <c r="B164" s="36"/>
-      <c r="C164" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="I163" s="28"/>
+    </row>
+    <row r="164" spans="1:10" ht="15.75">
+      <c r="A164" s="40">
+        <v>6</v>
+      </c>
+      <c r="B164" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C164" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D164" s="1"/>
       <c r="E164" s="1"/>
       <c r="F164" s="10"/>
       <c r="G164" s="10"/>
-      <c r="I164" s="29"/>
-    </row>
-    <row r="165" spans="1:140" ht="15.75">
-      <c r="A165" s="36"/>
-      <c r="B165" s="36"/>
-      <c r="C165" s="24" t="s">
-        <v>50</v>
+      <c r="I164" s="28"/>
+    </row>
+    <row r="165" spans="1:10" ht="15.75">
+      <c r="A165" s="40"/>
+      <c r="B165" s="40"/>
+      <c r="C165" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="D165" s="1"/>
-      <c r="E165" s="1"/>
+      <c r="E165" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F165" s="10"/>
       <c r="G165" s="10"/>
-      <c r="I165" s="29"/>
-    </row>
-    <row r="166" spans="1:140" ht="15.75">
-      <c r="A166" s="36"/>
-      <c r="B166" s="36"/>
-      <c r="C166" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="D166" s="1"/>
-      <c r="E166" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="I165" s="28"/>
+    </row>
+    <row r="166" spans="1:10" ht="15.75">
+      <c r="A166" s="40"/>
+      <c r="B166" s="40"/>
+      <c r="C166" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E166" s="1"/>
       <c r="F166" s="10"/>
       <c r="G166" s="10"/>
-      <c r="I166" s="29"/>
-    </row>
-    <row r="167" spans="1:140" ht="15.75">
-      <c r="A167" s="36"/>
-      <c r="B167" s="36"/>
-      <c r="C167" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="D167" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="I166" s="28"/>
+    </row>
+    <row r="167" spans="1:10" ht="15.75">
+      <c r="A167" s="40"/>
+      <c r="B167" s="40"/>
+      <c r="C167" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D167" s="1"/>
       <c r="E167" s="1"/>
       <c r="F167" s="10"/>
       <c r="G167" s="10"/>
-      <c r="I167" s="29"/>
-    </row>
-    <row r="168" spans="1:140" ht="15.75">
-      <c r="A168" s="36"/>
-      <c r="B168" s="36"/>
+      <c r="I167" s="28"/>
+    </row>
+    <row r="168" spans="1:10" ht="15.75">
+      <c r="A168" s="40"/>
+      <c r="B168" s="40"/>
       <c r="C168" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="D168" s="1"/>
-      <c r="E168" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E168" s="1"/>
       <c r="F168" s="10"/>
       <c r="G168" s="10"/>
-      <c r="I168" s="29"/>
-    </row>
-    <row r="169" spans="1:140" ht="15.75">
-      <c r="A169" s="36"/>
-      <c r="B169" s="36"/>
-      <c r="C169" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="D169" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="I168" s="28"/>
+    </row>
+    <row r="169" spans="1:10" ht="15.75">
+      <c r="A169" s="40"/>
+      <c r="B169" s="40"/>
+      <c r="C169" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D169" s="1"/>
       <c r="E169" s="1"/>
       <c r="F169" s="10"/>
       <c r="G169" s="10"/>
-      <c r="I169" s="29"/>
-    </row>
-    <row r="170" spans="1:140">
-      <c r="I170" s="29"/>
-    </row>
-    <row r="171" spans="1:140">
-      <c r="I171" s="29"/>
-    </row>
-    <row r="172" spans="1:140">
-      <c r="B172" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C172" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I172" s="29"/>
-    </row>
-    <row r="173" spans="1:140" ht="30">
-      <c r="B173" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C173" s="2">
-        <v>1</v>
-      </c>
-      <c r="I173" s="29"/>
-    </row>
-    <row r="174" spans="1:140" s="16" customFormat="1">
+      <c r="I169" s="28"/>
+    </row>
+    <row r="170" spans="1:10" ht="15.75">
+      <c r="A170" s="40"/>
+      <c r="B170" s="40"/>
+      <c r="C170" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="D170" s="1"/>
+      <c r="E170" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F170" s="10"/>
+      <c r="G170" s="10"/>
+      <c r="I170" s="28"/>
+    </row>
+    <row r="171" spans="1:10" ht="15.75">
+      <c r="A171" s="40"/>
+      <c r="B171" s="40"/>
+      <c r="C171" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E171" s="1"/>
+      <c r="F171" s="10"/>
+      <c r="G171" s="10"/>
+      <c r="I171" s="28"/>
+    </row>
+    <row r="172" spans="1:10" ht="15.75">
+      <c r="A172" s="40"/>
+      <c r="B172" s="40"/>
+      <c r="C172" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="D172" s="1"/>
+      <c r="E172" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F172" s="10"/>
+      <c r="G172" s="10"/>
+      <c r="I172" s="28"/>
+    </row>
+    <row r="173" spans="1:10" ht="15.75">
+      <c r="A173" s="40"/>
+      <c r="B173" s="40"/>
+      <c r="C173" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E173" s="1"/>
+      <c r="F173" s="10"/>
+      <c r="G173" s="10"/>
+      <c r="I173" s="28"/>
+    </row>
+    <row r="174" spans="1:10">
       <c r="A174" s="42"/>
-      <c r="B174" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C174" s="16">
-        <v>2</v>
-      </c>
+      <c r="B174" s="42"/>
+      <c r="C174" s="42"/>
       <c r="D174" s="42"/>
       <c r="E174" s="42"/>
       <c r="F174" s="42"/>
@@ -3548,268 +3595,305 @@
       <c r="H174" s="42"/>
       <c r="I174" s="42"/>
       <c r="J174" s="42"/>
-      <c r="K174" s="42"/>
-      <c r="L174" s="42"/>
-      <c r="M174" s="42"/>
-      <c r="N174" s="42"/>
-      <c r="O174" s="42"/>
-      <c r="P174" s="42"/>
-      <c r="Q174" s="42"/>
-      <c r="R174" s="42"/>
-      <c r="S174" s="42"/>
-      <c r="T174" s="42"/>
-      <c r="U174" s="42"/>
-      <c r="V174" s="42"/>
-      <c r="W174" s="42"/>
-      <c r="X174" s="42"/>
-      <c r="Y174" s="42"/>
-      <c r="Z174" s="42"/>
-      <c r="AA174" s="42"/>
-      <c r="AB174" s="42"/>
-      <c r="AC174" s="42"/>
-      <c r="AD174" s="42"/>
-      <c r="AE174" s="42"/>
-      <c r="AF174" s="42"/>
-      <c r="AG174" s="42"/>
-      <c r="AH174" s="42"/>
-      <c r="AI174" s="42"/>
-      <c r="AJ174" s="42"/>
-      <c r="AK174" s="42"/>
-      <c r="AL174" s="42"/>
-      <c r="AM174" s="42"/>
-      <c r="AN174" s="42"/>
-      <c r="AO174" s="42"/>
-      <c r="AP174" s="42"/>
-      <c r="AQ174" s="42"/>
-      <c r="AR174" s="42"/>
-      <c r="AS174" s="42"/>
-      <c r="AT174" s="42"/>
-      <c r="AU174" s="42"/>
-      <c r="AV174" s="42"/>
-      <c r="AW174" s="42"/>
-      <c r="AX174" s="42"/>
-      <c r="AY174" s="42"/>
-      <c r="AZ174" s="42"/>
-      <c r="BA174" s="42"/>
-      <c r="BB174" s="42"/>
-      <c r="BC174" s="42"/>
-      <c r="BD174" s="42"/>
-      <c r="BE174" s="42"/>
-      <c r="BF174" s="42"/>
-      <c r="BG174" s="42"/>
-      <c r="BH174" s="42"/>
-      <c r="BI174" s="42"/>
-      <c r="BJ174" s="42"/>
-      <c r="BK174" s="42"/>
-      <c r="BL174" s="42"/>
-      <c r="BM174" s="42"/>
-      <c r="BN174" s="42"/>
-      <c r="BO174" s="42"/>
-      <c r="BP174" s="42"/>
-      <c r="BQ174" s="42"/>
-      <c r="BR174" s="42"/>
-      <c r="BS174" s="42"/>
-      <c r="BT174" s="42"/>
-      <c r="BU174" s="42"/>
-      <c r="BV174" s="42"/>
-      <c r="BW174" s="42"/>
-      <c r="BX174" s="42"/>
-      <c r="BY174" s="42"/>
-      <c r="BZ174" s="42"/>
-      <c r="CA174" s="42"/>
-      <c r="CB174" s="42"/>
-      <c r="CC174" s="42"/>
-      <c r="CD174" s="42"/>
-      <c r="CE174" s="42"/>
-      <c r="CF174" s="42"/>
-      <c r="CG174" s="42"/>
-      <c r="CH174" s="42"/>
-      <c r="CI174" s="42"/>
-      <c r="CJ174" s="42"/>
-      <c r="CK174" s="42"/>
-      <c r="CL174" s="42"/>
-      <c r="CM174" s="42"/>
-      <c r="CN174" s="42"/>
-      <c r="CO174" s="42"/>
-      <c r="CP174" s="42"/>
-      <c r="CQ174" s="42"/>
-      <c r="CR174" s="42"/>
-      <c r="CS174" s="42"/>
-      <c r="CT174" s="42"/>
-      <c r="CU174" s="42"/>
-      <c r="CV174" s="42"/>
-      <c r="CW174" s="42"/>
-      <c r="CX174" s="42"/>
-      <c r="CY174" s="42"/>
-      <c r="CZ174" s="42"/>
-      <c r="DA174" s="42"/>
-      <c r="DB174" s="42"/>
-      <c r="DC174" s="42"/>
-      <c r="DD174" s="42"/>
-      <c r="DE174" s="42"/>
-      <c r="DF174" s="42"/>
-      <c r="DG174" s="42"/>
-      <c r="DH174" s="42"/>
-      <c r="DI174" s="42"/>
-      <c r="DJ174" s="42"/>
-      <c r="DK174" s="42"/>
-      <c r="DL174" s="42"/>
-      <c r="DM174" s="42"/>
-      <c r="DN174" s="42"/>
-      <c r="DO174" s="42"/>
-      <c r="DP174" s="42"/>
-      <c r="DQ174" s="42"/>
-      <c r="DR174" s="42"/>
-      <c r="DS174" s="42"/>
-      <c r="DT174" s="42"/>
-      <c r="DU174" s="42"/>
-      <c r="DV174" s="42"/>
-      <c r="DW174" s="42"/>
-      <c r="DX174" s="42"/>
-      <c r="DY174" s="42"/>
-      <c r="DZ174" s="42"/>
-      <c r="EA174" s="42"/>
-      <c r="EB174" s="42"/>
-      <c r="EC174" s="42"/>
-      <c r="ED174" s="42"/>
-      <c r="EE174" s="42"/>
-      <c r="EF174" s="42"/>
-      <c r="EG174" s="42"/>
-      <c r="EH174" s="42"/>
-      <c r="EI174" s="42"/>
-      <c r="EJ174" s="42"/>
-    </row>
-    <row r="175" spans="1:140">
-      <c r="B175" s="16" t="s">
+    </row>
+    <row r="175" spans="1:10">
+      <c r="I175" s="28"/>
+    </row>
+    <row r="176" spans="1:10">
+      <c r="B176" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I176" s="28"/>
+    </row>
+    <row r="177" spans="1:140" ht="30">
+      <c r="B177" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C177" s="2">
+        <v>1</v>
+      </c>
+      <c r="I177" s="28"/>
+    </row>
+    <row r="178" spans="1:140" s="16" customFormat="1">
+      <c r="A178" s="33"/>
+      <c r="B178" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C178" s="16">
+        <v>2</v>
+      </c>
+      <c r="D178" s="33"/>
+      <c r="E178" s="33"/>
+      <c r="F178" s="33"/>
+      <c r="G178" s="33"/>
+      <c r="H178" s="33"/>
+      <c r="I178" s="33"/>
+      <c r="J178" s="33"/>
+      <c r="K178" s="33"/>
+      <c r="L178" s="33"/>
+      <c r="M178" s="33"/>
+      <c r="N178" s="33"/>
+      <c r="O178" s="33"/>
+      <c r="P178" s="33"/>
+      <c r="Q178" s="33"/>
+      <c r="R178" s="33"/>
+      <c r="S178" s="33"/>
+      <c r="T178" s="33"/>
+      <c r="U178" s="33"/>
+      <c r="V178" s="33"/>
+      <c r="W178" s="33"/>
+      <c r="X178" s="33"/>
+      <c r="Y178" s="33"/>
+      <c r="Z178" s="33"/>
+      <c r="AA178" s="33"/>
+      <c r="AB178" s="33"/>
+      <c r="AC178" s="33"/>
+      <c r="AD178" s="33"/>
+      <c r="AE178" s="33"/>
+      <c r="AF178" s="33"/>
+      <c r="AG178" s="33"/>
+      <c r="AH178" s="33"/>
+      <c r="AI178" s="33"/>
+      <c r="AJ178" s="33"/>
+      <c r="AK178" s="33"/>
+      <c r="AL178" s="33"/>
+      <c r="AM178" s="33"/>
+      <c r="AN178" s="33"/>
+      <c r="AO178" s="33"/>
+      <c r="AP178" s="33"/>
+      <c r="AQ178" s="33"/>
+      <c r="AR178" s="33"/>
+      <c r="AS178" s="33"/>
+      <c r="AT178" s="33"/>
+      <c r="AU178" s="33"/>
+      <c r="AV178" s="33"/>
+      <c r="AW178" s="33"/>
+      <c r="AX178" s="33"/>
+      <c r="AY178" s="33"/>
+      <c r="AZ178" s="33"/>
+      <c r="BA178" s="33"/>
+      <c r="BB178" s="33"/>
+      <c r="BC178" s="33"/>
+      <c r="BD178" s="33"/>
+      <c r="BE178" s="33"/>
+      <c r="BF178" s="33"/>
+      <c r="BG178" s="33"/>
+      <c r="BH178" s="33"/>
+      <c r="BI178" s="33"/>
+      <c r="BJ178" s="33"/>
+      <c r="BK178" s="33"/>
+      <c r="BL178" s="33"/>
+      <c r="BM178" s="33"/>
+      <c r="BN178" s="33"/>
+      <c r="BO178" s="33"/>
+      <c r="BP178" s="33"/>
+      <c r="BQ178" s="33"/>
+      <c r="BR178" s="33"/>
+      <c r="BS178" s="33"/>
+      <c r="BT178" s="33"/>
+      <c r="BU178" s="33"/>
+      <c r="BV178" s="33"/>
+      <c r="BW178" s="33"/>
+      <c r="BX178" s="33"/>
+      <c r="BY178" s="33"/>
+      <c r="BZ178" s="33"/>
+      <c r="CA178" s="33"/>
+      <c r="CB178" s="33"/>
+      <c r="CC178" s="33"/>
+      <c r="CD178" s="33"/>
+      <c r="CE178" s="33"/>
+      <c r="CF178" s="33"/>
+      <c r="CG178" s="33"/>
+      <c r="CH178" s="33"/>
+      <c r="CI178" s="33"/>
+      <c r="CJ178" s="33"/>
+      <c r="CK178" s="33"/>
+      <c r="CL178" s="33"/>
+      <c r="CM178" s="33"/>
+      <c r="CN178" s="33"/>
+      <c r="CO178" s="33"/>
+      <c r="CP178" s="33"/>
+      <c r="CQ178" s="33"/>
+      <c r="CR178" s="33"/>
+      <c r="CS178" s="33"/>
+      <c r="CT178" s="33"/>
+      <c r="CU178" s="33"/>
+      <c r="CV178" s="33"/>
+      <c r="CW178" s="33"/>
+      <c r="CX178" s="33"/>
+      <c r="CY178" s="33"/>
+      <c r="CZ178" s="33"/>
+      <c r="DA178" s="33"/>
+      <c r="DB178" s="33"/>
+      <c r="DC178" s="33"/>
+      <c r="DD178" s="33"/>
+      <c r="DE178" s="33"/>
+      <c r="DF178" s="33"/>
+      <c r="DG178" s="33"/>
+      <c r="DH178" s="33"/>
+      <c r="DI178" s="33"/>
+      <c r="DJ178" s="33"/>
+      <c r="DK178" s="33"/>
+      <c r="DL178" s="33"/>
+      <c r="DM178" s="33"/>
+      <c r="DN178" s="33"/>
+      <c r="DO178" s="33"/>
+      <c r="DP178" s="33"/>
+      <c r="DQ178" s="33"/>
+      <c r="DR178" s="33"/>
+      <c r="DS178" s="33"/>
+      <c r="DT178" s="33"/>
+      <c r="DU178" s="33"/>
+      <c r="DV178" s="33"/>
+      <c r="DW178" s="33"/>
+      <c r="DX178" s="33"/>
+      <c r="DY178" s="33"/>
+      <c r="DZ178" s="33"/>
+      <c r="EA178" s="33"/>
+      <c r="EB178" s="33"/>
+      <c r="EC178" s="33"/>
+      <c r="ED178" s="33"/>
+      <c r="EE178" s="33"/>
+      <c r="EF178" s="33"/>
+      <c r="EG178" s="33"/>
+      <c r="EH178" s="33"/>
+      <c r="EI178" s="33"/>
+      <c r="EJ178" s="33"/>
+    </row>
+    <row r="179" spans="1:140">
+      <c r="B179" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C175" s="17">
+      <c r="C179" s="17">
         <v>3</v>
       </c>
-      <c r="I175" s="29"/>
-    </row>
-    <row r="176" spans="1:140">
-      <c r="B176" s="16" t="s">
+      <c r="I179" s="28"/>
+    </row>
+    <row r="180" spans="1:140">
+      <c r="B180" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C176" s="17">
+      <c r="C180" s="17">
         <v>4</v>
       </c>
-      <c r="I176" s="29"/>
-    </row>
-    <row r="177" spans="2:9">
-      <c r="B177" s="16" t="s">
+      <c r="I180" s="28"/>
+    </row>
+    <row r="181" spans="1:140">
+      <c r="B181" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C177" s="17">
+      <c r="C181" s="17">
         <v>5</v>
       </c>
-      <c r="I177" s="29"/>
-    </row>
-    <row r="178" spans="2:9">
-      <c r="I178" s="29"/>
-    </row>
-    <row r="179" spans="2:9">
-      <c r="I179" s="29"/>
-    </row>
-    <row r="180" spans="2:9">
-      <c r="I180" s="29"/>
-    </row>
-    <row r="181" spans="2:9">
-      <c r="I181" s="29"/>
-    </row>
-    <row r="182" spans="2:9">
-      <c r="I182" s="29"/>
-    </row>
-    <row r="183" spans="2:9">
-      <c r="I183" s="29"/>
-    </row>
-    <row r="184" spans="2:9">
-      <c r="I184" s="29"/>
-    </row>
-    <row r="185" spans="2:9">
-      <c r="I185" s="29"/>
-    </row>
-    <row r="186" spans="2:9">
-      <c r="I186" s="29"/>
-    </row>
-    <row r="187" spans="2:9">
-      <c r="I187" s="29"/>
-    </row>
-    <row r="188" spans="2:9">
-      <c r="I188" s="29"/>
-    </row>
-    <row r="189" spans="2:9">
-      <c r="I189" s="29"/>
-    </row>
-    <row r="190" spans="2:9">
-      <c r="I190" s="29"/>
-    </row>
-    <row r="191" spans="2:9">
-      <c r="I191" s="29"/>
-    </row>
-    <row r="192" spans="2:9">
-      <c r="I192" s="29"/>
+      <c r="I181" s="28"/>
+    </row>
+    <row r="182" spans="1:140">
+      <c r="I182" s="28"/>
+    </row>
+    <row r="183" spans="1:140">
+      <c r="I183" s="28"/>
+    </row>
+    <row r="184" spans="1:140">
+      <c r="I184" s="28"/>
+    </row>
+    <row r="185" spans="1:140">
+      <c r="I185" s="28"/>
+    </row>
+    <row r="186" spans="1:140">
+      <c r="I186" s="28"/>
+    </row>
+    <row r="187" spans="1:140">
+      <c r="I187" s="28"/>
+    </row>
+    <row r="188" spans="1:140">
+      <c r="I188" s="28"/>
+    </row>
+    <row r="189" spans="1:140">
+      <c r="I189" s="28"/>
+    </row>
+    <row r="190" spans="1:140">
+      <c r="I190" s="28"/>
+    </row>
+    <row r="191" spans="1:140">
+      <c r="I191" s="28"/>
+    </row>
+    <row r="192" spans="1:140">
+      <c r="I192" s="28"/>
     </row>
     <row r="193" spans="9:9">
-      <c r="I193" s="29"/>
+      <c r="I193" s="28"/>
     </row>
     <row r="194" spans="9:9">
-      <c r="I194" s="29"/>
+      <c r="I194" s="28"/>
     </row>
     <row r="195" spans="9:9">
-      <c r="I195" s="29"/>
+      <c r="I195" s="28"/>
     </row>
     <row r="196" spans="9:9">
-      <c r="I196" s="29"/>
+      <c r="I196" s="28"/>
     </row>
     <row r="197" spans="9:9">
-      <c r="I197" s="29"/>
+      <c r="I197" s="28"/>
     </row>
     <row r="198" spans="9:9">
-      <c r="I198" s="29"/>
+      <c r="I198" s="28"/>
     </row>
     <row r="199" spans="9:9">
-      <c r="I199" s="29"/>
+      <c r="I199" s="28"/>
     </row>
     <row r="200" spans="9:9">
-      <c r="I200" s="29"/>
+      <c r="I200" s="28"/>
     </row>
     <row r="201" spans="9:9">
-      <c r="I201" s="29"/>
+      <c r="I201" s="28"/>
     </row>
     <row r="202" spans="9:9">
-      <c r="I202" s="29"/>
+      <c r="I202" s="28"/>
     </row>
     <row r="203" spans="9:9">
-      <c r="I203" s="29"/>
+      <c r="I203" s="28"/>
     </row>
     <row r="204" spans="9:9">
-      <c r="I204" s="29"/>
+      <c r="I204" s="28"/>
     </row>
     <row r="205" spans="9:9">
-      <c r="I205" s="29"/>
+      <c r="I205" s="28"/>
     </row>
     <row r="206" spans="9:9">
-      <c r="I206" s="29"/>
+      <c r="I206" s="28"/>
+    </row>
+    <row r="207" spans="9:9">
+      <c r="I207" s="28"/>
+    </row>
+    <row r="208" spans="9:9">
+      <c r="I208" s="28"/>
+    </row>
+    <row r="209" spans="9:9">
+      <c r="I209" s="28"/>
+    </row>
+    <row r="210" spans="9:9">
+      <c r="I210" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B164:B173"/>
+    <mergeCell ref="A164:A173"/>
+    <mergeCell ref="B103:B163"/>
+    <mergeCell ref="A103:A163"/>
     <mergeCell ref="B8:B51"/>
     <mergeCell ref="A8:A51"/>
-    <mergeCell ref="B52:B100"/>
+    <mergeCell ref="B52:B102"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A52:A100"/>
-    <mergeCell ref="B160:B169"/>
-    <mergeCell ref="A160:A169"/>
-    <mergeCell ref="B101:B159"/>
-    <mergeCell ref="A101:A159"/>
+    <mergeCell ref="A52:A102"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E169">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E173">
       <formula1>"O, "</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>